<commit_message>
A bit more manual tagging done
</commit_message>
<xml_diff>
--- a/Results/CategorisationSummary.xlsx
+++ b/Results/CategorisationSummary.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755"/>
   </bookViews>
   <sheets>
     <sheet name="Emotions" sheetId="1" r:id="rId1"/>
@@ -13,16 +13,17 @@
     <sheet name="Summary" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Emotions!$A$1:$C$698</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">SideEffectStatus!$A$1:$C$160</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">SymptomSeverity!$A$1:$C$278</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3462" uniqueCount="1126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3491" uniqueCount="1140">
   <si>
     <t>Sentence</t>
   </si>
@@ -3409,6 +3410,48 @@
   </si>
   <si>
     <t>PostCount: 364</t>
+  </si>
+  <si>
+    <t>Complaint about the Doctors</t>
+  </si>
+  <si>
+    <t>Complaint not about the drug</t>
+  </si>
+  <si>
+    <t>More symptom related</t>
+  </si>
+  <si>
+    <t>Background of patient</t>
+  </si>
+  <si>
+    <t>Why did we not pick up drugs?</t>
+  </si>
+  <si>
+    <t>Drugs for side effects</t>
+  </si>
+  <si>
+    <t>Why have we not picked up side effects</t>
+  </si>
+  <si>
+    <t>Why did we not pick up symptoms</t>
+  </si>
+  <si>
+    <t>Why not picking up symptoms</t>
+  </si>
+  <si>
+    <t>Symptoms</t>
+  </si>
+  <si>
+    <t>Keyword side effect present</t>
+  </si>
+  <si>
+    <t>Tricky negation</t>
+  </si>
+  <si>
+    <t>Side effect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tricky use of negation </t>
   </si>
 </sst>
 </file>
@@ -3591,6 +3634,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -3638,7 +3684,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3673,7 +3719,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3882,20 +3928,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C698"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:F698"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="B69" workbookViewId="0">
+      <selection activeCell="E104" sqref="E104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3905,8 +3952,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>705</v>
+      </c>
+      <c r="F1" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -3916,8 +3969,11 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3927,8 +3983,11 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -3938,8 +3997,11 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -3949,8 +4011,11 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -3960,8 +4025,11 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -3971,8 +4039,11 @@
       <c r="C7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3982,8 +4053,11 @@
       <c r="C8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -3993,8 +4067,11 @@
       <c r="C9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -4005,7 +4082,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -4015,8 +4092,11 @@
       <c r="C11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -4026,8 +4106,14 @@
       <c r="C12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -4037,8 +4123,11 @@
       <c r="C13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -4048,8 +4137,11 @@
       <c r="C14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -4059,8 +4151,11 @@
       <c r="C15" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -4071,7 +4166,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -4081,8 +4176,11 @@
       <c r="C17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -4093,7 +4191,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -4104,7 +4202,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -4114,8 +4212,11 @@
       <c r="C20" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -4125,8 +4226,14 @@
       <c r="C21" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>748</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -4136,8 +4243,11 @@
       <c r="C22" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -4147,8 +4257,14 @@
       <c r="C23" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -4159,7 +4275,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -4169,8 +4285,14 @@
       <c r="C25" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>748</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -4180,8 +4302,11 @@
       <c r="C26" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -4191,8 +4316,11 @@
       <c r="C27" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -4203,7 +4331,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -4213,8 +4341,11 @@
       <c r="C29" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -4225,7 +4356,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -4236,7 +4367,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -4246,8 +4377,14 @@
       <c r="C32" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>748</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -4258,7 +4395,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -4269,7 +4406,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -4279,8 +4416,14 @@
       <c r="C35" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -4291,7 +4434,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -4302,7 +4445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -4313,7 +4456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -4324,7 +4467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -4334,8 +4477,14 @@
       <c r="C40" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E40" t="b">
+        <v>0</v>
+      </c>
+      <c r="F40" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -4346,7 +4495,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -4357,7 +4506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -4368,7 +4517,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -4379,7 +4528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -4390,7 +4539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -4401,7 +4550,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -4412,7 +4561,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -4423,7 +4572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -4434,7 +4583,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -4445,7 +4594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -4456,7 +4605,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -4467,7 +4616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>57</v>
       </c>
@@ -4478,7 +4627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -4488,8 +4637,11 @@
       <c r="C54" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -4499,8 +4651,11 @@
       <c r="C55" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -4510,8 +4665,11 @@
       <c r="C56" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -4521,8 +4679,11 @@
       <c r="C57" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>62</v>
       </c>
@@ -4532,8 +4693,11 @@
       <c r="C58" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -4543,8 +4707,11 @@
       <c r="C59" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -4554,8 +4721,14 @@
       <c r="C60" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E60" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>66</v>
       </c>
@@ -4566,7 +4739,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>67</v>
       </c>
@@ -4577,7 +4750,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>68</v>
       </c>
@@ -4588,7 +4761,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>69</v>
       </c>
@@ -4599,7 +4772,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>70</v>
       </c>
@@ -4610,7 +4783,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>71</v>
       </c>
@@ -4620,8 +4793,11 @@
       <c r="C66" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>72</v>
       </c>
@@ -4632,7 +4808,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>73</v>
       </c>
@@ -4643,7 +4819,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -4653,8 +4829,14 @@
       <c r="C69" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E69" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>75</v>
       </c>
@@ -4665,7 +4847,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>76</v>
       </c>
@@ -4675,8 +4857,14 @@
       <c r="C71" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E71" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>77</v>
       </c>
@@ -4686,8 +4874,14 @@
       <c r="C72" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E72" t="b">
+        <v>1</v>
+      </c>
+      <c r="F72" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>78</v>
       </c>
@@ -4698,7 +4892,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>79</v>
       </c>
@@ -4708,8 +4902,11 @@
       <c r="C74" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>80</v>
       </c>
@@ -4720,7 +4917,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>81</v>
       </c>
@@ -4731,7 +4928,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>82</v>
       </c>
@@ -4742,7 +4939,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>83</v>
       </c>
@@ -4752,8 +4949,11 @@
       <c r="C78" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>84</v>
       </c>
@@ -4764,7 +4964,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>85</v>
       </c>
@@ -4774,8 +4974,11 @@
       <c r="C80" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>86</v>
       </c>
@@ -4785,8 +4988,11 @@
       <c r="C81" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E81" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>87</v>
       </c>
@@ -4797,7 +5003,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>88</v>
       </c>
@@ -4808,7 +5014,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>89</v>
       </c>
@@ -4818,8 +5024,14 @@
       <c r="C84" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E84" t="b">
+        <v>0</v>
+      </c>
+      <c r="F84" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>90</v>
       </c>
@@ -4830,7 +5042,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>91</v>
       </c>
@@ -4841,7 +5053,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>92</v>
       </c>
@@ -4852,7 +5064,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>93</v>
       </c>
@@ -4862,8 +5074,11 @@
       <c r="C88" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E88" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>94</v>
       </c>
@@ -4874,7 +5089,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>95</v>
       </c>
@@ -4884,8 +5099,14 @@
       <c r="C90" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E90" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>96</v>
       </c>
@@ -4895,8 +5116,11 @@
       <c r="C91" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E91" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>97</v>
       </c>
@@ -4906,8 +5130,11 @@
       <c r="C92" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E92" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>98</v>
       </c>
@@ -4918,7 +5145,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>99</v>
       </c>
@@ -4928,8 +5155,11 @@
       <c r="C94" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>100</v>
       </c>
@@ -4940,7 +5170,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>101</v>
       </c>
@@ -4951,7 +5181,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>102</v>
       </c>
@@ -4962,7 +5192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>103</v>
       </c>
@@ -4973,7 +5203,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>104</v>
       </c>
@@ -4983,8 +5213,14 @@
       <c r="C99" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E99" t="s">
+        <v>748</v>
+      </c>
+      <c r="F99" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>105</v>
       </c>
@@ -4994,8 +5230,14 @@
       <c r="C100" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E100" t="b">
+        <v>0</v>
+      </c>
+      <c r="F100" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>106</v>
       </c>
@@ -5005,8 +5247,11 @@
       <c r="C101" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E101" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>107</v>
       </c>
@@ -5016,8 +5261,11 @@
       <c r="C102" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E102" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>108</v>
       </c>
@@ -5028,7 +5276,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>109</v>
       </c>
@@ -5039,7 +5287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>110</v>
       </c>
@@ -5050,7 +5298,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>111</v>
       </c>
@@ -5061,7 +5309,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>112</v>
       </c>
@@ -5072,7 +5320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>113</v>
       </c>
@@ -5083,7 +5331,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>114</v>
       </c>
@@ -5094,7 +5342,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>115</v>
       </c>
@@ -5105,7 +5353,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>116</v>
       </c>
@@ -5116,7 +5364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>117</v>
       </c>
@@ -5138,7 +5386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>119</v>
       </c>
@@ -5149,7 +5397,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>120</v>
       </c>
@@ -5160,7 +5408,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>121</v>
       </c>
@@ -5204,7 +5452,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>125</v>
       </c>
@@ -5259,7 +5507,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>130</v>
       </c>
@@ -5281,7 +5529,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>132</v>
       </c>
@@ -5336,7 +5584,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>137</v>
       </c>
@@ -5347,7 +5595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>138</v>
       </c>
@@ -5380,7 +5628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>141</v>
       </c>
@@ -5402,7 +5650,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>143</v>
       </c>
@@ -5501,7 +5749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>152</v>
       </c>
@@ -5523,7 +5771,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>154</v>
       </c>
@@ -5534,7 +5782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>155</v>
       </c>
@@ -5556,7 +5804,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>157</v>
       </c>
@@ -5600,7 +5848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>161</v>
       </c>
@@ -5644,7 +5892,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>165</v>
       </c>
@@ -5677,7 +5925,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>168</v>
       </c>
@@ -5688,7 +5936,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>169</v>
       </c>
@@ -5710,7 +5958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>171</v>
       </c>
@@ -5754,7 +6002,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>175</v>
       </c>
@@ -5798,7 +6046,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>179</v>
       </c>
@@ -5809,7 +6057,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>180</v>
       </c>
@@ -5820,7 +6068,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>181</v>
       </c>
@@ -5831,7 +6079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>182</v>
       </c>
@@ -5897,7 +6145,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>188</v>
       </c>
@@ -5908,7 +6156,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>189</v>
       </c>
@@ -5919,7 +6167,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>190</v>
       </c>
@@ -5952,7 +6200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>193</v>
       </c>
@@ -5963,7 +6211,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>194</v>
       </c>
@@ -5974,7 +6222,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>195</v>
       </c>
@@ -5985,7 +6233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>196</v>
       </c>
@@ -6007,7 +6255,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>198</v>
       </c>
@@ -6029,7 +6277,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>200</v>
       </c>
@@ -6040,7 +6288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>201</v>
       </c>
@@ -6084,7 +6332,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>205</v>
       </c>
@@ -6095,7 +6343,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>206</v>
       </c>
@@ -6106,7 +6354,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>207</v>
       </c>
@@ -6117,7 +6365,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>208</v>
       </c>
@@ -6128,7 +6376,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>209</v>
       </c>
@@ -6139,7 +6387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>210</v>
       </c>
@@ -6194,7 +6442,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>215</v>
       </c>
@@ -6227,7 +6475,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>218</v>
       </c>
@@ -6249,7 +6497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>220</v>
       </c>
@@ -6271,7 +6519,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>222</v>
       </c>
@@ -6282,7 +6530,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>223</v>
       </c>
@@ -6293,7 +6541,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>224</v>
       </c>
@@ -6348,7 +6596,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>229</v>
       </c>
@@ -6359,7 +6607,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>230</v>
       </c>
@@ -6370,7 +6618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>231</v>
       </c>
@@ -6392,7 +6640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>233</v>
       </c>
@@ -6403,7 +6651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>234</v>
       </c>
@@ -6414,7 +6662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>235</v>
       </c>
@@ -6425,7 +6673,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>236</v>
       </c>
@@ -6447,7 +6695,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>238</v>
       </c>
@@ -6458,7 +6706,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="234" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>239</v>
       </c>
@@ -6469,7 +6717,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>240</v>
       </c>
@@ -6480,7 +6728,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>241</v>
       </c>
@@ -6491,7 +6739,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>242</v>
       </c>
@@ -6502,7 +6750,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>243</v>
       </c>
@@ -6513,7 +6761,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>244</v>
       </c>
@@ -6524,7 +6772,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>245</v>
       </c>
@@ -6535,7 +6783,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>246</v>
       </c>
@@ -6546,7 +6794,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>247</v>
       </c>
@@ -6557,7 +6805,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>248</v>
       </c>
@@ -6568,7 +6816,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="244" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>249</v>
       </c>
@@ -6590,7 +6838,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>251</v>
       </c>
@@ -6656,7 +6904,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>257</v>
       </c>
@@ -6678,7 +6926,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>259</v>
       </c>
@@ -6711,7 +6959,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>262</v>
       </c>
@@ -6722,7 +6970,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>263</v>
       </c>
@@ -6733,7 +6981,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>264</v>
       </c>
@@ -6744,7 +6992,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>265</v>
       </c>
@@ -6766,7 +7014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>267</v>
       </c>
@@ -6777,7 +7025,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>268</v>
       </c>
@@ -6865,7 +7113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>276</v>
       </c>
@@ -6887,7 +7135,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>278</v>
       </c>
@@ -6898,7 +7146,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>279</v>
       </c>
@@ -6909,7 +7157,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>280</v>
       </c>
@@ -6920,7 +7168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>281</v>
       </c>
@@ -6953,7 +7201,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>284</v>
       </c>
@@ -6964,7 +7212,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>285</v>
       </c>
@@ -7019,7 +7267,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>290</v>
       </c>
@@ -7030,7 +7278,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>291</v>
       </c>
@@ -7085,7 +7333,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>296</v>
       </c>
@@ -7096,7 +7344,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>297</v>
       </c>
@@ -7129,7 +7377,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>300</v>
       </c>
@@ -7162,7 +7410,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>303</v>
       </c>
@@ -7173,7 +7421,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>304</v>
       </c>
@@ -7228,7 +7476,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>309</v>
       </c>
@@ -7261,7 +7509,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>312</v>
       </c>
@@ -7272,7 +7520,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>313</v>
       </c>
@@ -7283,7 +7531,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>314</v>
       </c>
@@ -7327,7 +7575,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>318</v>
       </c>
@@ -7349,7 +7597,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>320</v>
       </c>
@@ -7360,7 +7608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>321</v>
       </c>
@@ -7371,7 +7619,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>322</v>
       </c>
@@ -7382,7 +7630,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>323</v>
       </c>
@@ -7426,7 +7674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>327</v>
       </c>
@@ -7481,7 +7729,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>332</v>
       </c>
@@ -7514,7 +7762,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>335</v>
       </c>
@@ -7525,7 +7773,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>336</v>
       </c>
@@ -7602,7 +7850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="338" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>343</v>
       </c>
@@ -7613,7 +7861,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="339" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>344</v>
       </c>
@@ -7657,7 +7905,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="343" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>348</v>
       </c>
@@ -7668,7 +7916,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="344" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>349</v>
       </c>
@@ -7690,7 +7938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="346" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>351</v>
       </c>
@@ -7712,7 +7960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="348" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>353</v>
       </c>
@@ -7723,7 +7971,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="349" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>354</v>
       </c>
@@ -7734,7 +7982,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="350" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>355</v>
       </c>
@@ -7756,7 +8004,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="352" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>357</v>
       </c>
@@ -7767,7 +8015,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="353" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>358</v>
       </c>
@@ -7778,7 +8026,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="354" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>359</v>
       </c>
@@ -7800,7 +8048,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="356" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>361</v>
       </c>
@@ -7811,7 +8059,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="357" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>362</v>
       </c>
@@ -7833,7 +8081,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="359" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>364</v>
       </c>
@@ -7844,7 +8092,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="360" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>365</v>
       </c>
@@ -7855,7 +8103,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="361" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>366</v>
       </c>
@@ -7866,7 +8114,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="362" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>367</v>
       </c>
@@ -7888,7 +8136,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>369</v>
       </c>
@@ -7910,7 +8158,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="366" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>371</v>
       </c>
@@ -7943,7 +8191,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="369" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>374</v>
       </c>
@@ -7954,7 +8202,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="370" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>375</v>
       </c>
@@ -7976,7 +8224,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="372" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>377</v>
       </c>
@@ -7987,7 +8235,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="373" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>378</v>
       </c>
@@ -8009,7 +8257,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="375" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>380</v>
       </c>
@@ -8064,7 +8312,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="380" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>385</v>
       </c>
@@ -8075,7 +8323,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="381" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>386</v>
       </c>
@@ -8119,7 +8367,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>390</v>
       </c>
@@ -8130,7 +8378,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>391</v>
       </c>
@@ -8141,7 +8389,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>392</v>
       </c>
@@ -8163,7 +8411,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>394</v>
       </c>
@@ -8174,7 +8422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>395</v>
       </c>
@@ -8185,7 +8433,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>396</v>
       </c>
@@ -8240,7 +8488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>401</v>
       </c>
@@ -8262,7 +8510,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>403</v>
       </c>
@@ -8306,7 +8554,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="402" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>407</v>
       </c>
@@ -8372,7 +8620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="408" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>413</v>
       </c>
@@ -8438,7 +8686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="414" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>419</v>
       </c>
@@ -8548,7 +8796,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="424" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>429</v>
       </c>
@@ -8603,7 +8851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="429" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>434</v>
       </c>
@@ -8625,7 +8873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="431" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>436</v>
       </c>
@@ -8691,7 +8939,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="437" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>442</v>
       </c>
@@ -8702,7 +8950,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="438" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>443</v>
       </c>
@@ -8746,7 +8994,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="442" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>447</v>
       </c>
@@ -8812,7 +9060,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="448" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>453</v>
       </c>
@@ -8878,7 +9126,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="454" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>459</v>
       </c>
@@ -8900,7 +9148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="456" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
         <v>461</v>
       </c>
@@ -8944,7 +9192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="460" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
         <v>465</v>
       </c>
@@ -8966,7 +9214,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="462" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
         <v>467</v>
       </c>
@@ -8977,7 +9225,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="463" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>468</v>
       </c>
@@ -8988,7 +9236,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="464" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
         <v>469</v>
       </c>
@@ -8999,7 +9247,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="465" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
         <v>470</v>
       </c>
@@ -9021,7 +9269,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="467" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
         <v>472</v>
       </c>
@@ -9043,7 +9291,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="469" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
         <v>474</v>
       </c>
@@ -9098,7 +9346,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="474" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
         <v>479</v>
       </c>
@@ -9142,7 +9390,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="478" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
         <v>483</v>
       </c>
@@ -9153,7 +9401,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="479" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
         <v>484</v>
       </c>
@@ -9164,7 +9412,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="480" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
         <v>485</v>
       </c>
@@ -9175,7 +9423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="481" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
         <v>486</v>
       </c>
@@ -9241,7 +9489,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="487" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
         <v>492</v>
       </c>
@@ -9263,7 +9511,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="489" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
         <v>494</v>
       </c>
@@ -9285,7 +9533,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="491" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
         <v>496</v>
       </c>
@@ -9318,7 +9566,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="494" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
         <v>499</v>
       </c>
@@ -9351,7 +9599,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="497" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
         <v>502</v>
       </c>
@@ -9362,7 +9610,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="498" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
         <v>503</v>
       </c>
@@ -9395,7 +9643,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="501" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
         <v>506</v>
       </c>
@@ -9406,7 +9654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="502" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
         <v>507</v>
       </c>
@@ -9417,7 +9665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="503" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
         <v>508</v>
       </c>
@@ -9494,7 +9742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="510" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
         <v>515</v>
       </c>
@@ -9505,7 +9753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="511" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
         <v>516</v>
       </c>
@@ -9516,7 +9764,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="512" spans="1:3" ht="345" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A512" s="1" t="s">
         <v>517</v>
       </c>
@@ -9527,7 +9775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="513" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
         <v>518</v>
       </c>
@@ -9538,7 +9786,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="514" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
         <v>519</v>
       </c>
@@ -9549,7 +9797,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="515" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
         <v>520</v>
       </c>
@@ -9582,7 +9830,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="518" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
         <v>523</v>
       </c>
@@ -9604,7 +9852,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="520" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
         <v>525</v>
       </c>
@@ -9615,7 +9863,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="521" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
         <v>526</v>
       </c>
@@ -9626,7 +9874,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="522" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
         <v>527</v>
       </c>
@@ -9659,7 +9907,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="525" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
         <v>530</v>
       </c>
@@ -9670,7 +9918,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="526" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
         <v>531</v>
       </c>
@@ -9714,7 +9962,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="530" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
         <v>535</v>
       </c>
@@ -9747,7 +9995,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="533" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
         <v>538</v>
       </c>
@@ -9758,7 +10006,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="534" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
         <v>539</v>
       </c>
@@ -9769,7 +10017,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="535" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
         <v>540</v>
       </c>
@@ -9780,7 +10028,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="536" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
         <v>541</v>
       </c>
@@ -9791,7 +10039,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="537" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
         <v>542</v>
       </c>
@@ -9879,7 +10127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="545" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="545" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A545" t="s">
         <v>550</v>
       </c>
@@ -9890,7 +10138,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="546" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="546" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
         <v>551</v>
       </c>
@@ -9901,7 +10149,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="547" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
         <v>552</v>
       </c>
@@ -9923,7 +10171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="549" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="549" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
         <v>554</v>
       </c>
@@ -9934,7 +10182,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="550" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="550" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
         <v>555</v>
       </c>
@@ -9967,7 +10215,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="553" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="553" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
         <v>558</v>
       </c>
@@ -9978,7 +10226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="554" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="554" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A554" t="s">
         <v>559</v>
       </c>
@@ -9989,7 +10237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="555" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
         <v>560</v>
       </c>
@@ -10000,7 +10248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="556" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="556" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A556" t="s">
         <v>561</v>
       </c>
@@ -10033,7 +10281,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="559" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="559" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
         <v>564</v>
       </c>
@@ -10044,7 +10292,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="560" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="560" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
         <v>565</v>
       </c>
@@ -10077,7 +10325,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="563" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="563" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A563" t="s">
         <v>568</v>
       </c>
@@ -10143,7 +10391,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="569" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="569" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A569" t="s">
         <v>574</v>
       </c>
@@ -10165,7 +10413,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="571" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="571" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A571" t="s">
         <v>576</v>
       </c>
@@ -10220,7 +10468,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="576" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="576" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A576" t="s">
         <v>581</v>
       </c>
@@ -10253,7 +10501,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="579" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="579" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A579" t="s">
         <v>584</v>
       </c>
@@ -10264,7 +10512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="580" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="580" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A580" t="s">
         <v>585</v>
       </c>
@@ -10275,7 +10523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="581" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="581" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
         <v>586</v>
       </c>
@@ -10286,7 +10534,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="582" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="582" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A582" t="s">
         <v>587</v>
       </c>
@@ -10297,7 +10545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="583" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="583" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
         <v>588</v>
       </c>
@@ -10308,7 +10556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="584" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="584" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A584" t="s">
         <v>589</v>
       </c>
@@ -10319,7 +10567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="585" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="585" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A585" t="s">
         <v>590</v>
       </c>
@@ -10374,7 +10622,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="590" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="590" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A590" t="s">
         <v>595</v>
       </c>
@@ -10385,7 +10633,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="591" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="591" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A591" t="s">
         <v>596</v>
       </c>
@@ -10396,7 +10644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="592" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="592" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A592" t="s">
         <v>597</v>
       </c>
@@ -10451,7 +10699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="597" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="597" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A597" t="s">
         <v>602</v>
       </c>
@@ -10484,7 +10732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="600" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="600" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A600" t="s">
         <v>605</v>
       </c>
@@ -10550,7 +10798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="606" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="606" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A606" t="s">
         <v>611</v>
       </c>
@@ -10594,7 +10842,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="610" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="610" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A610" t="s">
         <v>615</v>
       </c>
@@ -10616,7 +10864,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="612" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="612" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A612" t="s">
         <v>617</v>
       </c>
@@ -10649,7 +10897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="615" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="615" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A615" t="s">
         <v>620</v>
       </c>
@@ -10660,7 +10908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="616" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="616" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A616" t="s">
         <v>621</v>
       </c>
@@ -10671,7 +10919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="617" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="617" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A617" t="s">
         <v>622</v>
       </c>
@@ -10682,7 +10930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="618" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="618" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A618" t="s">
         <v>623</v>
       </c>
@@ -10693,7 +10941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="619" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="619" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A619" t="s">
         <v>624</v>
       </c>
@@ -10704,7 +10952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="620" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="620" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A620" t="s">
         <v>625</v>
       </c>
@@ -10737,7 +10985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="623" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="623" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A623" t="s">
         <v>628</v>
       </c>
@@ -10748,7 +10996,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="624" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="624" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A624" t="s">
         <v>629</v>
       </c>
@@ -10770,7 +11018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="626" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="626" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A626" t="s">
         <v>631</v>
       </c>
@@ -10781,7 +11029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="627" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="627" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A627" t="s">
         <v>632</v>
       </c>
@@ -10792,7 +11040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="628" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="628" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A628" t="s">
         <v>633</v>
       </c>
@@ -10803,7 +11051,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="629" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="629" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A629" t="s">
         <v>634</v>
       </c>
@@ -10858,7 +11106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="634" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="634" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A634" t="s">
         <v>639</v>
       </c>
@@ -10869,7 +11117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="635" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="635" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A635" t="s">
         <v>640</v>
       </c>
@@ -10880,7 +11128,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="636" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="636" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A636" t="s">
         <v>641</v>
       </c>
@@ -10913,7 +11161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="639" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="639" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A639" t="s">
         <v>644</v>
       </c>
@@ -10968,7 +11216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="644" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="644" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A644" t="s">
         <v>649</v>
       </c>
@@ -10990,7 +11238,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="646" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="646" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A646" t="s">
         <v>651</v>
       </c>
@@ -11001,7 +11249,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="647" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="647" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A647" t="s">
         <v>652</v>
       </c>
@@ -11023,7 +11271,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="649" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+    <row r="649" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A649" s="1" t="s">
         <v>654</v>
       </c>
@@ -11034,7 +11282,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="650" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="650" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A650" s="1" t="s">
         <v>655</v>
       </c>
@@ -11045,7 +11293,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="651" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="651" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A651" t="s">
         <v>656</v>
       </c>
@@ -11078,7 +11326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="654" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="654" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A654" t="s">
         <v>659</v>
       </c>
@@ -11089,7 +11337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="655" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="655" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A655" t="s">
         <v>660</v>
       </c>
@@ -11100,7 +11348,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="656" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="656" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A656" t="s">
         <v>661</v>
       </c>
@@ -11111,7 +11359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="657" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="657" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A657" t="s">
         <v>662</v>
       </c>
@@ -11133,7 +11381,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="659" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="659" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A659" t="s">
         <v>664</v>
       </c>
@@ -11144,7 +11392,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="660" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="660" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A660" t="s">
         <v>665</v>
       </c>
@@ -11155,7 +11403,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="661" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="661" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A661" t="s">
         <v>666</v>
       </c>
@@ -11276,7 +11524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="672" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="672" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A672" t="s">
         <v>677</v>
       </c>
@@ -11298,7 +11546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="674" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="674" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A674" t="s">
         <v>679</v>
       </c>
@@ -11320,7 +11568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="676" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="676" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A676" t="s">
         <v>681</v>
       </c>
@@ -11364,7 +11612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="680" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="680" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A680" t="s">
         <v>685</v>
       </c>
@@ -11375,7 +11623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="681" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="681" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A681" t="s">
         <v>686</v>
       </c>
@@ -11386,7 +11634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="682" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="682" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A682" t="s">
         <v>687</v>
       </c>
@@ -11397,7 +11645,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="683" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="683" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A683" t="s">
         <v>688</v>
       </c>
@@ -11452,7 +11700,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="688" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="688" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A688" t="s">
         <v>693</v>
       </c>
@@ -11463,7 +11711,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="689" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="689" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A689" t="s">
         <v>694</v>
       </c>
@@ -11485,7 +11733,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="691" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="691" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A691" t="s">
         <v>696</v>
       </c>
@@ -11507,7 +11755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="693" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="693" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A693" t="s">
         <v>698</v>
       </c>
@@ -11518,7 +11766,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="694" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="694" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A694" t="s">
         <v>699</v>
       </c>
@@ -11529,7 +11777,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="695" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="695" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A695" t="s">
         <v>700</v>
       </c>
@@ -11540,7 +11788,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="696" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="696" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A696" t="s">
         <v>701</v>
       </c>
@@ -11551,7 +11799,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="697" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="697" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A697" t="s">
         <v>702</v>
       </c>
@@ -11562,7 +11810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="698" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="698" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A698" t="s">
         <v>703</v>
       </c>
@@ -11574,6 +11822,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C698">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Negative Experience - No symptoms mentioned but negative words found"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -11583,7 +11838,7 @@
   <dimension ref="A1:F160"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="E1" sqref="E1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12631,7 +12886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>801</v>
       </c>
@@ -15694,7 +15949,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>801</v>
       </c>
@@ -16796,8 +17051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16863,32 +17118,32 @@
         <v>318</v>
       </c>
       <c r="E2" s="4">
-        <f xml:space="preserve"> COUNTIFS(Emotions!$B$2:$B$698, B2, Emotions!$D$2:$D$698, "=TRUE" )</f>
-        <v>0</v>
+        <f xml:space="preserve"> COUNTIFS(Emotions!$B$2:$B$698, B2, Emotions!$E$2:$E$698, "=TRUE" )</f>
+        <v>3</v>
       </c>
       <c r="F2" s="4">
-        <f xml:space="preserve"> COUNTIFS(Emotions!$B$2:$B$698, C2, Emotions!$D$2:$D$698, "=FALSE" )</f>
-        <v>0</v>
+        <f xml:space="preserve"> COUNTIFS(Emotions!$B$2:$B$698, B2, Emotions!$E$2:$E$698, "=FALSE" )</f>
+        <v>1</v>
       </c>
       <c r="G2" s="5">
-        <f xml:space="preserve"> COUNTIFS(Emotions!$B$2:$B$698, D2, Emotions!$D$2:$D$698, "=NA" )</f>
-        <v>0</v>
+        <f xml:space="preserve"> COUNTIFS(Emotions!$B$2:$B$698, B2, Emotions!$E$2:$E$698, "=NA" )</f>
+        <v>1</v>
       </c>
       <c r="I2">
         <f xml:space="preserve"> ($E2/$D2)*100</f>
-        <v>0</v>
+        <v>0.94339622641509435</v>
       </c>
       <c r="J2">
         <f xml:space="preserve"> ($F2/$D2)*100</f>
-        <v>0</v>
+        <v>0.31446540880503149</v>
       </c>
       <c r="K2">
         <f xml:space="preserve"> ($G2/$D2)*100</f>
-        <v>0</v>
+        <v>0.31446540880503149</v>
       </c>
       <c r="M2">
         <f>(SUM($E2:$G2) /$D2) * 100</f>
-        <v>0</v>
+        <v>1.5723270440251573</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -16904,32 +17159,32 @@
         <v>379</v>
       </c>
       <c r="E3" s="7">
-        <f xml:space="preserve"> COUNTIFS(Emotions!$B$2:$B$698, B3, Emotions!$D$2:$D$698, "=TRUE" )</f>
-        <v>0</v>
+        <f xml:space="preserve"> COUNTIFS(Emotions!$B$2:$B$698, B3, Emotions!$E$2:$E$698, "=TRUE" )</f>
+        <v>27</v>
       </c>
       <c r="F3" s="7">
-        <f xml:space="preserve"> COUNTIFS(Emotions!$B$2:$B$698, C3, Emotions!$D$2:$D$698, "=FALSE" )</f>
-        <v>0</v>
+        <f xml:space="preserve"> COUNTIFS(Emotions!$B$2:$B$698, B3, Emotions!$E$2:$E$698, "=FALSE" )</f>
+        <v>7</v>
       </c>
       <c r="G3" s="8">
-        <f xml:space="preserve"> COUNTIFS(Emotions!$B$2:$B$698, D3, Emotions!$D$2:$D$698, "=NA" )</f>
-        <v>0</v>
+        <f xml:space="preserve"> COUNTIFS(Emotions!$B$2:$B$698, B3, Emotions!$E$2:$E$698, "=NA" )</f>
+        <v>11</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I10" si="0" xml:space="preserve"> ($E3/$D3)*100</f>
-        <v>0</v>
+        <v>7.1240105540897103</v>
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J10" si="1" xml:space="preserve"> ($F3/$D3)*100</f>
-        <v>0</v>
+        <v>1.8469656992084433</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K10" si="2" xml:space="preserve"> ($G3/$D3)*100</f>
-        <v>0</v>
+        <v>2.9023746701846966</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="J3:M10" si="3">(SUM($E3:$G3) /$D3) * 100</f>
-        <v>0</v>
+        <f t="shared" ref="M3:M10" si="3">(SUM($E3:$G3) /$D3) * 100</f>
+        <v>11.87335092348285</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added more drugs to the postsGatherer and did some more tagging in the result
</commit_message>
<xml_diff>
--- a/Results/CategorisationSummary.xlsx
+++ b/Results/CategorisationSummary.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Emotions" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">SymptomSeverity!$A$1:$C$278</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3491" uniqueCount="1140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3509" uniqueCount="1144">
   <si>
     <t>Sentence</t>
   </si>
@@ -3452,6 +3452,18 @@
   </si>
   <si>
     <t xml:space="preserve">Tricky use of negation </t>
+  </si>
+  <si>
+    <t>Symptom related</t>
+  </si>
+  <si>
+    <t>Very true comment</t>
+  </si>
+  <si>
+    <t>Complain about doctors</t>
+  </si>
+  <si>
+    <t>Bith of both</t>
   </si>
 </sst>
 </file>
@@ -3684,7 +3696,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3719,7 +3731,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3931,15 +3943,16 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F698"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B69" workbookViewId="0">
-      <selection activeCell="E104" sqref="E104"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E165" sqref="E165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="143" customWidth="1"/>
+    <col min="2" max="2" width="70.42578125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -5286,6 +5299,12 @@
       <c r="C104" t="s">
         <v>5</v>
       </c>
+      <c r="E104" t="b">
+        <v>1</v>
+      </c>
+      <c r="F104" t="s">
+        <v>1140</v>
+      </c>
     </row>
     <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
@@ -5308,6 +5327,9 @@
       <c r="C106" t="s">
         <v>5</v>
       </c>
+      <c r="E106" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
@@ -5330,6 +5352,9 @@
       <c r="C108" t="s">
         <v>5</v>
       </c>
+      <c r="E108" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
@@ -5341,6 +5366,9 @@
       <c r="C109" t="s">
         <v>5</v>
       </c>
+      <c r="E109" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
@@ -5352,6 +5380,12 @@
       <c r="C110" t="s">
         <v>5</v>
       </c>
+      <c r="E110" t="b">
+        <v>1</v>
+      </c>
+      <c r="F110" t="s">
+        <v>1140</v>
+      </c>
     </row>
     <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
@@ -5375,7 +5409,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>118</v>
       </c>
@@ -5385,8 +5419,11 @@
       <c r="C113" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E113" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>119</v>
       </c>
@@ -5397,7 +5434,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>120</v>
       </c>
@@ -5408,7 +5445,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>121</v>
       </c>
@@ -5419,7 +5456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>122</v>
       </c>
@@ -5429,8 +5466,11 @@
       <c r="C117" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E117" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>123</v>
       </c>
@@ -5440,8 +5480,11 @@
       <c r="C118" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E118" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>124</v>
       </c>
@@ -5451,8 +5494,14 @@
       <c r="C119" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E119" t="b">
+        <v>1</v>
+      </c>
+      <c r="F119" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>125</v>
       </c>
@@ -5463,7 +5512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>126</v>
       </c>
@@ -5473,8 +5522,11 @@
       <c r="C121" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E121" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>127</v>
       </c>
@@ -5484,8 +5536,11 @@
       <c r="C122" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E122" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>128</v>
       </c>
@@ -5495,8 +5550,11 @@
       <c r="C123" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E123" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>129</v>
       </c>
@@ -5506,8 +5564,11 @@
       <c r="C124" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E124" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>130</v>
       </c>
@@ -5518,7 +5579,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>131</v>
       </c>
@@ -5528,8 +5589,11 @@
       <c r="C126" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E126" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>132</v>
       </c>
@@ -5540,7 +5604,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>133</v>
       </c>
@@ -5550,8 +5614,11 @@
       <c r="C128" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E128" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>134</v>
       </c>
@@ -5561,8 +5628,11 @@
       <c r="C129" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E129" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>135</v>
       </c>
@@ -5572,8 +5642,14 @@
       <c r="C130" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E130" t="b">
+        <v>0</v>
+      </c>
+      <c r="F130" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>136</v>
       </c>
@@ -5583,8 +5659,11 @@
       <c r="C131" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E131" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>137</v>
       </c>
@@ -5595,7 +5674,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>138</v>
       </c>
@@ -5606,7 +5685,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>139</v>
       </c>
@@ -5616,8 +5695,11 @@
       <c r="C134" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E134" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>140</v>
       </c>
@@ -5627,8 +5709,11 @@
       <c r="C135" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E135" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>141</v>
       </c>
@@ -5639,7 +5724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>142</v>
       </c>
@@ -5649,8 +5734,11 @@
       <c r="C137" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E137" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>143</v>
       </c>
@@ -5661,7 +5749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>144</v>
       </c>
@@ -5671,8 +5759,11 @@
       <c r="C139" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E139" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>145</v>
       </c>
@@ -5682,8 +5773,14 @@
       <c r="C140" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E140" t="b">
+        <v>1</v>
+      </c>
+      <c r="F140" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>146</v>
       </c>
@@ -5693,8 +5790,11 @@
       <c r="C141" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E141" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>147</v>
       </c>
@@ -5704,8 +5804,14 @@
       <c r="C142" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E142" t="b">
+        <v>1</v>
+      </c>
+      <c r="F142" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>148</v>
       </c>
@@ -5715,8 +5821,14 @@
       <c r="C143" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E143" t="b">
+        <v>1</v>
+      </c>
+      <c r="F143" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>149</v>
       </c>
@@ -5726,8 +5838,14 @@
       <c r="C144" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E144" t="s">
+        <v>748</v>
+      </c>
+      <c r="F144" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>150</v>
       </c>
@@ -5737,8 +5855,11 @@
       <c r="C145" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E145" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>151</v>
       </c>
@@ -5748,8 +5869,14 @@
       <c r="C146" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E146" t="b">
+        <v>1</v>
+      </c>
+      <c r="F146" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>152</v>
       </c>
@@ -5760,7 +5887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>153</v>
       </c>
@@ -5770,8 +5897,11 @@
       <c r="C148" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E148" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>154</v>
       </c>
@@ -5782,7 +5912,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>155</v>
       </c>
@@ -5793,7 +5923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>156</v>
       </c>
@@ -5803,8 +5933,14 @@
       <c r="C151" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E151" t="s">
+        <v>748</v>
+      </c>
+      <c r="F151" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>157</v>
       </c>
@@ -5815,7 +5951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>158</v>
       </c>
@@ -5825,8 +5961,14 @@
       <c r="C153" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E153" t="b">
+        <v>1</v>
+      </c>
+      <c r="F153" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>159</v>
       </c>
@@ -5836,8 +5978,11 @@
       <c r="C154" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E154" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>160</v>
       </c>
@@ -5847,8 +5992,11 @@
       <c r="C155" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E155" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>161</v>
       </c>
@@ -5859,7 +6007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>162</v>
       </c>
@@ -5870,7 +6018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>163</v>
       </c>
@@ -5881,7 +6029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>164</v>
       </c>
@@ -5892,7 +6040,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>165</v>
       </c>
@@ -11838,7 +11986,7 @@
   <dimension ref="A1:F160"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13736,7 +13884,7 @@
   <dimension ref="A1:F278"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17051,8 +17199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17160,31 +17308,31 @@
       </c>
       <c r="E3" s="7">
         <f xml:space="preserve"> COUNTIFS(Emotions!$B$2:$B$698, B3, Emotions!$E$2:$E$698, "=TRUE" )</f>
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="F3" s="7">
         <f xml:space="preserve"> COUNTIFS(Emotions!$B$2:$B$698, B3, Emotions!$E$2:$E$698, "=FALSE" )</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G3" s="8">
         <f xml:space="preserve"> COUNTIFS(Emotions!$B$2:$B$698, B3, Emotions!$E$2:$E$698, "=NA" )</f>
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I10" si="0" xml:space="preserve"> ($E3/$D3)*100</f>
-        <v>7.1240105540897103</v>
+        <v>13.456464379947231</v>
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J10" si="1" xml:space="preserve"> ($F3/$D3)*100</f>
-        <v>1.8469656992084433</v>
+        <v>2.6385224274406331</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K10" si="2" xml:space="preserve"> ($G3/$D3)*100</f>
-        <v>2.9023746701846966</v>
+        <v>4.7493403693931393</v>
       </c>
       <c r="M3">
         <f t="shared" ref="M3:M10" si="3">(SUM($E3:$G3) /$D3) * 100</f>
-        <v>11.87335092348285</v>
+        <v>20.844327176781004</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>